<commit_message>
1. Loop estimates and plots for both SE and NI, for both SCE and SPF. 2. The results of reported in the note for meeting with Jonathan.
</commit_message>
<xml_diff>
--- a/workingfolder/python/tables/NI_Est.xlsx
+++ b/workingfolder/python/tables/NI_Est.xlsx
@@ -477,13 +477,13 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>98.52</v>
+        <v>4.17</v>
       </c>
       <c r="F2">
-        <v>1.69</v>
+        <v>164.56</v>
       </c>
       <c r="G2">
-        <v>0.2</v>
+        <v>10.51</v>
       </c>
       <c r="H2">
         <v>0.5</v>
@@ -501,10 +501,10 @@
         <v>0.1</v>
       </c>
       <c r="M2">
-        <v>98.52</v>
+        <v>-0.34</v>
       </c>
       <c r="N2">
-        <v>1.69</v>
+        <v>32.02</v>
       </c>
       <c r="O2">
         <v>0.2</v>
@@ -530,10 +530,10 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>151.59</v>
+        <v>-2.15</v>
       </c>
       <c r="F3">
-        <v>0.95</v>
+        <v>167.73</v>
       </c>
       <c r="G3">
         <v>0.2</v>
@@ -554,10 +554,10 @@
         <v>0.1</v>
       </c>
       <c r="M3">
-        <v>151.59</v>
+        <v>1.38</v>
       </c>
       <c r="N3">
-        <v>0.95</v>
+        <v>-0.46</v>
       </c>
       <c r="O3">
         <v>0.2</v>
@@ -586,10 +586,10 @@
         <v>8</v>
       </c>
       <c r="E4">
-        <v>-0.7</v>
+        <v>205.05</v>
       </c>
       <c r="F4">
-        <v>336.37</v>
+        <v>1.52</v>
       </c>
       <c r="G4">
         <v>0.2</v>
@@ -610,10 +610,10 @@
         <v>0.1</v>
       </c>
       <c r="M4">
-        <v>-0.7</v>
+        <v>0.47</v>
       </c>
       <c r="N4">
-        <v>336.37</v>
+        <v>0.35</v>
       </c>
       <c r="O4">
         <v>0.2</v>
@@ -645,13 +645,13 @@
         <v>9</v>
       </c>
       <c r="E5">
-        <v>1.63</v>
+        <v>9.57</v>
       </c>
       <c r="F5">
-        <v>115.06</v>
+        <v>3.58</v>
       </c>
       <c r="G5">
-        <v>0.2</v>
+        <v>1.51</v>
       </c>
       <c r="H5">
         <v>0.5</v>
@@ -669,13 +669,13 @@
         <v>0.1</v>
       </c>
       <c r="M5">
-        <v>1.63</v>
+        <v>1043.13</v>
       </c>
       <c r="N5">
-        <v>115.06</v>
+        <v>11.08</v>
       </c>
       <c r="O5">
-        <v>0.2</v>
+        <v>640.86</v>
       </c>
       <c r="P5">
         <v>0.5</v>
@@ -707,10 +707,10 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>-0.63</v>
+        <v>76.29000000000001</v>
       </c>
       <c r="F6">
-        <v>131.43</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="G6">
         <v>0.2</v>
@@ -731,13 +731,13 @@
         <v>0.1</v>
       </c>
       <c r="M6">
-        <v>-0.63</v>
+        <v>2682.64</v>
       </c>
       <c r="N6">
-        <v>131.43</v>
+        <v>334.37</v>
       </c>
       <c r="O6">
-        <v>0.2</v>
+        <v>14227.79</v>
       </c>
       <c r="P6">
         <v>0.5</v>
@@ -752,7 +752,7 @@
         <v>0.8</v>
       </c>
       <c r="T6">
-        <v>0.1</v>
+        <v>1.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Loop estimates with bounds.So NI for SPF is now more stable. Problems that need to be addressed: 1. add a constant to SCE. 2. try autocovariance instead.
</commit_message>
<xml_diff>
--- a/workingfolder/python/tables/NI_Est.xlsx
+++ b/workingfolder/python/tables/NI_Est.xlsx
@@ -477,13 +477,13 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>4.17</v>
+        <v>376.66</v>
       </c>
       <c r="F2">
-        <v>164.56</v>
+        <v>1.26</v>
       </c>
       <c r="G2">
-        <v>10.51</v>
+        <v>0.1</v>
       </c>
       <c r="H2">
         <v>0.5</v>
@@ -501,13 +501,13 @@
         <v>0.1</v>
       </c>
       <c r="M2">
-        <v>-0.34</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>32.02</v>
+        <v>1.13</v>
       </c>
       <c r="O2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="P2">
         <v>0.5</v>
@@ -530,13 +530,13 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>-2.15</v>
+        <v>1.04</v>
       </c>
       <c r="F3">
-        <v>167.73</v>
+        <v>159.74</v>
       </c>
       <c r="G3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H3">
         <v>0.5</v>
@@ -554,13 +554,13 @@
         <v>0.1</v>
       </c>
       <c r="M3">
-        <v>1.38</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>-0.46</v>
+        <v>1.26</v>
       </c>
       <c r="O3">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="P3">
         <v>0.5</v>
@@ -586,13 +586,13 @@
         <v>8</v>
       </c>
       <c r="E4">
-        <v>205.05</v>
+        <v>1.14</v>
       </c>
       <c r="F4">
-        <v>1.52</v>
+        <v>6.74</v>
       </c>
       <c r="G4">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H4">
         <v>0.5</v>
@@ -610,13 +610,13 @@
         <v>0.1</v>
       </c>
       <c r="M4">
-        <v>0.47</v>
+        <v>0.59</v>
       </c>
       <c r="N4">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
       <c r="O4">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="P4">
         <v>0.5</v>
@@ -645,13 +645,13 @@
         <v>9</v>
       </c>
       <c r="E5">
-        <v>9.57</v>
+        <v>1.39</v>
       </c>
       <c r="F5">
-        <v>3.58</v>
+        <v>1.46</v>
       </c>
       <c r="G5">
-        <v>1.51</v>
+        <v>0.1</v>
       </c>
       <c r="H5">
         <v>0.5</v>
@@ -669,13 +669,13 @@
         <v>0.1</v>
       </c>
       <c r="M5">
-        <v>1043.13</v>
+        <v>2354.37</v>
       </c>
       <c r="N5">
-        <v>11.08</v>
+        <v>10.93</v>
       </c>
       <c r="O5">
-        <v>640.86</v>
+        <v>113.65</v>
       </c>
       <c r="P5">
         <v>0.5</v>
@@ -707,13 +707,13 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>76.29000000000001</v>
+        <v>1.37</v>
       </c>
       <c r="F6">
-        <v>0.6899999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="G6">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H6">
         <v>0.5</v>
@@ -731,13 +731,13 @@
         <v>0.1</v>
       </c>
       <c r="M6">
-        <v>2682.64</v>
+        <v>35263.31</v>
       </c>
       <c r="N6">
-        <v>334.37</v>
+        <v>332.04</v>
       </c>
       <c r="O6">
-        <v>14227.79</v>
+        <v>14197.41</v>
       </c>
       <c r="P6">
         <v>0.5</v>
@@ -752,7 +752,7 @@
         <v>0.8</v>
       </c>
       <c r="T6">
-        <v>1.1</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NIAR estimation is redone for SPF and SCE with crazily large estimates. May need to rethink moments. Need to add diff-scale for joint. Joint has problom.Need to think about autocovariance.
</commit_message>
<xml_diff>
--- a/workingfolder/python/tables/NI_Est.xlsx
+++ b/workingfolder/python/tables/NI_Est.xlsx
@@ -477,13 +477,13 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>376.66</v>
+        <v>1975.32</v>
       </c>
       <c r="F2">
-        <v>1.26</v>
+        <v>147.49</v>
       </c>
       <c r="G2">
-        <v>0.1</v>
+        <v>1273.05</v>
       </c>
       <c r="H2">
         <v>0.5</v>
@@ -495,16 +495,16 @@
         <v>0.1</v>
       </c>
       <c r="K2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>0.1</v>
       </c>
       <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
         <v>0</v>
-      </c>
-      <c r="N2">
-        <v>1.13</v>
       </c>
       <c r="O2">
         <v>0.5</v>
@@ -530,13 +530,13 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>1.04</v>
+        <v>72.18000000000001</v>
       </c>
       <c r="F3">
-        <v>159.74</v>
+        <v>1737.21</v>
       </c>
       <c r="G3">
-        <v>0.1</v>
+        <v>523.89</v>
       </c>
       <c r="H3">
         <v>0.5</v>
@@ -548,16 +548,16 @@
         <v>0.1</v>
       </c>
       <c r="K3">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>0.1</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="N3">
-        <v>1.26</v>
+        <v>0.99</v>
       </c>
       <c r="O3">
         <v>0.5</v>
@@ -586,13 +586,13 @@
         <v>8</v>
       </c>
       <c r="E4">
-        <v>1.14</v>
+        <v>67.22</v>
       </c>
       <c r="F4">
-        <v>6.74</v>
+        <v>631.79</v>
       </c>
       <c r="G4">
-        <v>0.1</v>
+        <v>430.11</v>
       </c>
       <c r="H4">
         <v>0.5</v>
@@ -604,16 +604,16 @@
         <v>0.1</v>
       </c>
       <c r="K4">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <v>0.1</v>
       </c>
       <c r="M4">
-        <v>0.59</v>
+        <v>1.27</v>
       </c>
       <c r="N4">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="O4">
         <v>0.5</v>
@@ -645,13 +645,13 @@
         <v>9</v>
       </c>
       <c r="E5">
-        <v>1.39</v>
+        <v>39.18</v>
       </c>
       <c r="F5">
-        <v>1.46</v>
+        <v>424.69</v>
       </c>
       <c r="G5">
-        <v>0.1</v>
+        <v>92738.05</v>
       </c>
       <c r="H5">
         <v>0.5</v>
@@ -663,19 +663,19 @@
         <v>0.1</v>
       </c>
       <c r="K5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <v>0.1</v>
       </c>
       <c r="M5">
-        <v>2354.37</v>
+        <v>1702.06</v>
       </c>
       <c r="N5">
-        <v>10.93</v>
+        <v>11.05</v>
       </c>
       <c r="O5">
-        <v>113.65</v>
+        <v>49.7</v>
       </c>
       <c r="P5">
         <v>0.5</v>
@@ -707,13 +707,13 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>1.37</v>
+        <v>4.57</v>
       </c>
       <c r="F6">
-        <v>1.1</v>
+        <v>3.19</v>
       </c>
       <c r="G6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0.5</v>
@@ -725,19 +725,19 @@
         <v>0.1</v>
       </c>
       <c r="K6">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <v>0.1</v>
       </c>
       <c r="M6">
-        <v>35263.31</v>
+        <v>176791.47</v>
       </c>
       <c r="N6">
-        <v>332.04</v>
+        <v>332</v>
       </c>
       <c r="O6">
-        <v>14197.41</v>
+        <v>14191.81</v>
       </c>
       <c r="P6">
         <v>0.5</v>

</xml_diff>

<commit_message>
include diff_scale feature for all in AR estimate.
</commit_message>
<xml_diff>
--- a/workingfolder/python/tables/NI_Est.xlsx
+++ b/workingfolder/python/tables/NI_Est.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
   <si>
     <t>NI: $\hat\sigma_{pb,SPF}$</t>
   </si>
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -477,13 +477,13 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>1975.32</v>
+        <v>197.7</v>
       </c>
       <c r="F2">
-        <v>147.49</v>
+        <v>6011.89</v>
       </c>
       <c r="G2">
-        <v>1273.05</v>
+        <v>1959.51</v>
       </c>
       <c r="H2">
         <v>0.5</v>
@@ -501,10 +501,10 @@
         <v>0.1</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>0.82</v>
       </c>
       <c r="O2">
         <v>0.5</v>
@@ -530,13 +530,13 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>72.18000000000001</v>
+        <v>75.01000000000001</v>
       </c>
       <c r="F3">
-        <v>1737.21</v>
+        <v>3278.5</v>
       </c>
       <c r="G3">
-        <v>523.89</v>
+        <v>2632.47</v>
       </c>
       <c r="H3">
         <v>0.5</v>
@@ -554,10 +554,10 @@
         <v>0.1</v>
       </c>
       <c r="M3">
-        <v>0.34</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>0.99</v>
+        <v>1.21</v>
       </c>
       <c r="O3">
         <v>0.5</v>
@@ -586,13 +586,13 @@
         <v>8</v>
       </c>
       <c r="E4">
-        <v>67.22</v>
+        <v>4841.28</v>
       </c>
       <c r="F4">
-        <v>631.79</v>
+        <v>166.01</v>
       </c>
       <c r="G4">
-        <v>430.11</v>
+        <v>1953.53</v>
       </c>
       <c r="H4">
         <v>0.5</v>
@@ -610,10 +610,10 @@
         <v>0.1</v>
       </c>
       <c r="M4">
-        <v>1.27</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1.17</v>
       </c>
       <c r="O4">
         <v>0.5</v>
@@ -645,13 +645,13 @@
         <v>9</v>
       </c>
       <c r="E5">
-        <v>39.18</v>
+        <v>45.21</v>
       </c>
       <c r="F5">
-        <v>424.69</v>
+        <v>556.33</v>
       </c>
       <c r="G5">
-        <v>92738.05</v>
+        <v>185448.25</v>
       </c>
       <c r="H5">
         <v>0.5</v>
@@ -669,13 +669,13 @@
         <v>0.1</v>
       </c>
       <c r="M5">
-        <v>1702.06</v>
+        <v>1703.7</v>
       </c>
       <c r="N5">
-        <v>11.05</v>
+        <v>10.94</v>
       </c>
       <c r="O5">
-        <v>49.7</v>
+        <v>60.61</v>
       </c>
       <c r="P5">
         <v>0.5</v>
@@ -707,13 +707,13 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>4.57</v>
+        <v>2.28</v>
       </c>
       <c r="F6">
-        <v>3.19</v>
+        <v>18.79</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1.36</v>
       </c>
       <c r="H6">
         <v>0.5</v>
@@ -731,13 +731,13 @@
         <v>0.1</v>
       </c>
       <c r="M6">
-        <v>176791.47</v>
+        <v>9150.26</v>
       </c>
       <c r="N6">
-        <v>332</v>
+        <v>332.08</v>
       </c>
       <c r="O6">
-        <v>14191.81</v>
+        <v>14172.03</v>
       </c>
       <c r="P6">
         <v>0.5</v>
@@ -752,6 +752,62 @@
         <v>0.8</v>
       </c>
       <c r="T6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>90.12</v>
+      </c>
+      <c r="F7">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.1</v>
+      </c>
+      <c r="H7">
+        <v>0.5</v>
+      </c>
+      <c r="I7">
+        <v>0.5</v>
+      </c>
+      <c r="J7">
+        <v>0.1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0.1</v>
+      </c>
+      <c r="M7">
+        <v>3297.11</v>
+      </c>
+      <c r="N7">
+        <v>333.49</v>
+      </c>
+      <c r="O7">
+        <v>14198.59</v>
+      </c>
+      <c r="P7">
+        <v>0.5</v>
+      </c>
+      <c r="Q7">
+        <v>0.5</v>
+      </c>
+      <c r="R7">
+        <v>0.1</v>
+      </c>
+      <c r="S7">
+        <v>0.8</v>
+      </c>
+      <c r="T7">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rewrote the draft of the GMMEst note to include results for SV as well as the theoretical derivations of the SV model.
</commit_message>
<xml_diff>
--- a/workingfolder/python/tables/NI_Est.xlsx
+++ b/workingfolder/python/tables/NI_Est.xlsx
@@ -477,13 +477,13 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>197.7</v>
+        <v>5.64</v>
       </c>
       <c r="F2">
-        <v>6011.89</v>
+        <v>804.51</v>
       </c>
       <c r="G2">
-        <v>1959.51</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0.5</v>
@@ -501,10 +501,10 @@
         <v>0.1</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>93.17</v>
       </c>
       <c r="N2">
-        <v>0.82</v>
+        <v>0.64</v>
       </c>
       <c r="O2">
         <v>0.5</v>
@@ -530,13 +530,13 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>75.01000000000001</v>
+        <v>2197.33</v>
       </c>
       <c r="F3">
-        <v>3278.5</v>
+        <v>60.45</v>
       </c>
       <c r="G3">
-        <v>2632.47</v>
+        <v>1283.2</v>
       </c>
       <c r="H3">
         <v>0.5</v>
@@ -554,10 +554,10 @@
         <v>0.1</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="N3">
-        <v>1.21</v>
+        <v>0.34</v>
       </c>
       <c r="O3">
         <v>0.5</v>
@@ -586,13 +586,13 @@
         <v>8</v>
       </c>
       <c r="E4">
-        <v>4841.28</v>
+        <v>8565.83</v>
       </c>
       <c r="F4">
-        <v>166.01</v>
+        <v>176.23</v>
       </c>
       <c r="G4">
-        <v>1953.53</v>
+        <v>2019.63</v>
       </c>
       <c r="H4">
         <v>0.5</v>
@@ -610,10 +610,10 @@
         <v>0.1</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="N4">
-        <v>1.17</v>
+        <v>0.44</v>
       </c>
       <c r="O4">
         <v>0.5</v>
@@ -645,13 +645,13 @@
         <v>9</v>
       </c>
       <c r="E5">
-        <v>45.21</v>
+        <v>30.39</v>
       </c>
       <c r="F5">
-        <v>556.33</v>
+        <v>353.42</v>
       </c>
       <c r="G5">
-        <v>185448.25</v>
+        <v>22189.31</v>
       </c>
       <c r="H5">
         <v>0.5</v>
@@ -669,13 +669,13 @@
         <v>0.1</v>
       </c>
       <c r="M5">
-        <v>1703.7</v>
+        <v>3154.03</v>
       </c>
       <c r="N5">
-        <v>10.94</v>
+        <v>10.93</v>
       </c>
       <c r="O5">
-        <v>60.61</v>
+        <v>117.33</v>
       </c>
       <c r="P5">
         <v>0.5</v>
@@ -707,13 +707,13 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>2.28</v>
+        <v>2.43</v>
       </c>
       <c r="F6">
-        <v>18.79</v>
+        <v>63.03</v>
       </c>
       <c r="G6">
-        <v>1.36</v>
+        <v>8.109999999999999</v>
       </c>
       <c r="H6">
         <v>0.5</v>
@@ -731,13 +731,13 @@
         <v>0.1</v>
       </c>
       <c r="M6">
-        <v>9150.26</v>
+        <v>22970.9</v>
       </c>
       <c r="N6">
-        <v>332.08</v>
+        <v>332.03</v>
       </c>
       <c r="O6">
-        <v>14172.03</v>
+        <v>14193.59</v>
       </c>
       <c r="P6">
         <v>0.5</v>

</xml_diff>

<commit_message>
slides for brown bag seminar. Will work on following things. 1. true GMM, unconditional moments. 2. randseed lead to SMM.
</commit_message>
<xml_diff>
--- a/workingfolder/python/tables/NI_Est.xlsx
+++ b/workingfolder/python/tables/NI_Est.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>NI: $\hat\sigma_{pb,SPF}$</t>
   </si>
@@ -23,12 +23,6 @@
   </si>
   <si>
     <t>$Var$</t>
-  </si>
-  <si>
-    <t>NI: $\rho$</t>
-  </si>
-  <si>
-    <t>NI: $\sigma$</t>
   </si>
   <si>
     <t>NI: $\hat\sigma_{pb,SCE}$</t>
@@ -404,13 +398,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:9">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -420,395 +414,150 @@
       <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" t="s">
-        <v>7</v>
+      <c r="D2">
+        <v>39.65</v>
       </c>
       <c r="E2">
-        <v>5.64</v>
+        <v>192.22</v>
       </c>
       <c r="F2">
-        <v>804.51</v>
+        <v>44.97</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>2.35</v>
       </c>
       <c r="H2">
-        <v>0.5</v>
+        <v>0.38</v>
       </c>
       <c r="I2">
         <v>0.5</v>
       </c>
-      <c r="J2">
-        <v>0.1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>0.1</v>
-      </c>
-      <c r="M2">
-        <v>93.17</v>
-      </c>
-      <c r="N2">
-        <v>0.64</v>
-      </c>
-      <c r="O2">
-        <v>0.5</v>
-      </c>
-      <c r="P2">
-        <v>0.5</v>
-      </c>
-      <c r="Q2">
-        <v>0.5</v>
-      </c>
-      <c r="R2">
-        <v>0.1</v>
-      </c>
-      <c r="S2">
-        <v>0.8</v>
-      </c>
-      <c r="T2">
-        <v>0.1</v>
-      </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>12.64</v>
       </c>
       <c r="E3">
-        <v>2197.33</v>
+        <v>211.14</v>
       </c>
       <c r="F3">
-        <v>60.45</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>1283.2</v>
+        <v>1.64</v>
       </c>
       <c r="H3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <v>0.5</v>
       </c>
-      <c r="J3">
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>112.37</v>
+      </c>
+      <c r="E4">
+        <v>0.34</v>
+      </c>
+      <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>0.1</v>
-      </c>
-      <c r="M3">
-        <v>0.62</v>
-      </c>
-      <c r="N3">
-        <v>0.34</v>
-      </c>
-      <c r="O3">
-        <v>0.5</v>
-      </c>
-      <c r="P3">
-        <v>0.5</v>
-      </c>
-      <c r="Q3">
-        <v>0.5</v>
-      </c>
-      <c r="R3">
-        <v>0.1</v>
-      </c>
-      <c r="S3">
-        <v>0.8</v>
-      </c>
-      <c r="T3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>8565.83</v>
-      </c>
-      <c r="F4">
-        <v>176.23</v>
-      </c>
       <c r="G4">
-        <v>2019.63</v>
+        <v>512.51</v>
       </c>
       <c r="H4">
-        <v>0.5</v>
+        <v>0.86</v>
       </c>
       <c r="I4">
         <v>0.5</v>
       </c>
-      <c r="J4">
-        <v>0.1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>0.1</v>
-      </c>
-      <c r="M4">
-        <v>0.62</v>
-      </c>
-      <c r="N4">
-        <v>0.44</v>
-      </c>
-      <c r="O4">
-        <v>0.5</v>
-      </c>
-      <c r="P4">
-        <v>0.5</v>
-      </c>
-      <c r="Q4">
-        <v>0.5</v>
-      </c>
-      <c r="R4">
-        <v>0.1</v>
-      </c>
-      <c r="S4">
-        <v>0.8</v>
-      </c>
-      <c r="T4">
-        <v>0.1</v>
-      </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
+      <c r="D5">
+        <v>1.13</v>
       </c>
       <c r="E5">
-        <v>30.39</v>
+        <v>367.43</v>
       </c>
       <c r="F5">
-        <v>353.42</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>22189.31</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.5</v>
+        <v>1.28</v>
       </c>
       <c r="I5">
         <v>0.5</v>
       </c>
-      <c r="J5">
-        <v>0.1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>0.1</v>
-      </c>
-      <c r="M5">
-        <v>3154.03</v>
-      </c>
-      <c r="N5">
-        <v>10.93</v>
-      </c>
-      <c r="O5">
-        <v>117.33</v>
-      </c>
-      <c r="P5">
-        <v>0.5</v>
-      </c>
-      <c r="Q5">
-        <v>0.5</v>
-      </c>
-      <c r="R5">
-        <v>0.1</v>
-      </c>
-      <c r="S5">
-        <v>0.8</v>
-      </c>
-      <c r="T5">
-        <v>0.1</v>
-      </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
+      <c r="D6">
+        <v>1.29</v>
       </c>
       <c r="E6">
-        <v>2.43</v>
+        <v>29.84</v>
       </c>
       <c r="F6">
-        <v>63.03</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>8.109999999999999</v>
+        <v>2.74</v>
       </c>
       <c r="H6">
-        <v>0.5</v>
+        <v>127.86</v>
       </c>
       <c r="I6">
         <v>0.5</v>
-      </c>
-      <c r="J6">
-        <v>0.1</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>0.1</v>
-      </c>
-      <c r="M6">
-        <v>22970.9</v>
-      </c>
-      <c r="N6">
-        <v>332.03</v>
-      </c>
-      <c r="O6">
-        <v>14193.59</v>
-      </c>
-      <c r="P6">
-        <v>0.5</v>
-      </c>
-      <c r="Q6">
-        <v>0.5</v>
-      </c>
-      <c r="R6">
-        <v>0.1</v>
-      </c>
-      <c r="S6">
-        <v>0.8</v>
-      </c>
-      <c r="T6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>90.12</v>
-      </c>
-      <c r="F7">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="G7">
-        <v>0.1</v>
-      </c>
-      <c r="H7">
-        <v>0.5</v>
-      </c>
-      <c r="I7">
-        <v>0.5</v>
-      </c>
-      <c r="J7">
-        <v>0.1</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>0.1</v>
-      </c>
-      <c r="M7">
-        <v>3297.11</v>
-      </c>
-      <c r="N7">
-        <v>333.49</v>
-      </c>
-      <c r="O7">
-        <v>14198.59</v>
-      </c>
-      <c r="P7">
-        <v>0.5</v>
-      </c>
-      <c r="Q7">
-        <v>0.5</v>
-      </c>
-      <c r="R7">
-        <v>0.1</v>
-      </c>
-      <c r="S7">
-        <v>0.8</v>
-      </c>
-      <c r="T7">
-        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a1. add np.random.seed to the simulate signals for NI estimation in GMMEst.ipynb so that each time the estimation is the same. 2. working on GMMEst_dev to do unditional moments, and to do SMM.
</commit_message>
<xml_diff>
--- a/workingfolder/python/tables/NI_Est.xlsx
+++ b/workingfolder/python/tables/NI_Est.xlsx
@@ -438,19 +438,19 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>39.65</v>
+        <v>66.04000000000001</v>
       </c>
       <c r="E2">
-        <v>192.22</v>
+        <v>297.94</v>
       </c>
       <c r="F2">
-        <v>44.97</v>
+        <v>72.86</v>
       </c>
       <c r="G2">
-        <v>2.35</v>
+        <v>31.86</v>
       </c>
       <c r="H2">
-        <v>0.38</v>
+        <v>0.53</v>
       </c>
       <c r="I2">
         <v>0.5</v>
@@ -461,19 +461,19 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>12.64</v>
+        <v>1.44</v>
       </c>
       <c r="E3">
-        <v>211.14</v>
+        <v>0.16</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G3">
-        <v>1.64</v>
+        <v>106.35</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1.15</v>
       </c>
       <c r="I3">
         <v>0.5</v>
@@ -487,19 +487,19 @@
         <v>7</v>
       </c>
       <c r="D4">
-        <v>112.37</v>
+        <v>1.48</v>
       </c>
       <c r="E4">
-        <v>0.34</v>
+        <v>0.16</v>
       </c>
       <c r="F4">
         <v>0.1</v>
       </c>
       <c r="G4">
-        <v>512.51</v>
+        <v>153.58</v>
       </c>
       <c r="H4">
-        <v>0.86</v>
+        <v>1.21</v>
       </c>
       <c r="I4">
         <v>0.5</v>
@@ -513,19 +513,19 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <v>1.13</v>
+        <v>72.31999999999999</v>
       </c>
       <c r="E5">
-        <v>367.43</v>
+        <v>0.16</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>160.16</v>
       </c>
       <c r="H5">
-        <v>1.28</v>
+        <v>1.23</v>
       </c>
       <c r="I5">
         <v>0.5</v>
@@ -542,19 +542,19 @@
         <v>8</v>
       </c>
       <c r="D6">
-        <v>1.29</v>
+        <v>81.2</v>
       </c>
       <c r="E6">
-        <v>29.84</v>
+        <v>0.16</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G6">
-        <v>2.74</v>
+        <v>137.65</v>
       </c>
       <c r="H6">
-        <v>127.86</v>
+        <v>1.28</v>
       </c>
       <c r="I6">
         <v>0.5</v>

</xml_diff>

<commit_message>
1. first round of results with SMM. mostly work. need to clean up the difference between -dev and orginal files.
</commit_message>
<xml_diff>
--- a/workingfolder/python/tables/NI_Est.xlsx
+++ b/workingfolder/python/tables/NI_Est.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>NI: $\hat\sigma_{pb,SPF}$</t>
   </si>
@@ -22,7 +22,10 @@
     <t>$\hat\sigma_{pr,SPF}$</t>
   </si>
   <si>
-    <t>$Var$</t>
+    <t>NI: $\rho$</t>
+  </si>
+  <si>
+    <t>NI: $\sigma$</t>
   </si>
   <si>
     <t>NI: $\hat\sigma_{pb,SCE}$</t>
@@ -31,13 +34,16 @@
     <t>$\hat\sigma_{pr,SCE}$</t>
   </si>
   <si>
-    <t>Forecast</t>
-  </si>
-  <si>
-    <t>FE</t>
-  </si>
-  <si>
-    <t>Disg</t>
+    <t>FEVar</t>
+  </si>
+  <si>
+    <t>DisgVar</t>
+  </si>
+  <si>
+    <t>FEATV</t>
+  </si>
+  <si>
+    <t>DisgATV</t>
   </si>
   <si>
     <t>Var</t>
@@ -398,13 +404,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:17">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -414,150 +420,238 @@
       <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>66.04000000000001</v>
-      </c>
-      <c r="E2">
-        <v>297.94</v>
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
       <c r="F2">
-        <v>72.86</v>
+        <v>25.32</v>
       </c>
       <c r="G2">
-        <v>31.86</v>
+        <v>16.07</v>
       </c>
       <c r="H2">
-        <v>0.53</v>
+        <v>0.9</v>
       </c>
       <c r="I2">
-        <v>0.5</v>
+        <v>1.09</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>3.4</v>
+      </c>
+      <c r="M2">
+        <v>15.4</v>
+      </c>
+      <c r="N2">
+        <v>3.4</v>
+      </c>
+      <c r="O2">
+        <v>11.29</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>1.44</v>
-      </c>
-      <c r="E3">
-        <v>0.16</v>
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
       <c r="F3">
-        <v>0.1</v>
+        <v>471301.73</v>
       </c>
       <c r="G3">
-        <v>106.35</v>
+        <v>0.85</v>
       </c>
       <c r="H3">
-        <v>1.15</v>
+        <v>-1.74</v>
       </c>
       <c r="I3">
-        <v>0.5</v>
+        <v>-0.17</v>
+      </c>
+      <c r="J3">
+        <v>0.91</v>
+      </c>
+      <c r="K3">
+        <v>0.42</v>
+      </c>
+      <c r="L3">
+        <v>168519.46</v>
+      </c>
+      <c r="M3">
+        <v>1.09</v>
+      </c>
+      <c r="N3">
+        <v>0.67</v>
+      </c>
+      <c r="O3">
+        <v>0.58</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
-        <v>1.48</v>
-      </c>
-      <c r="E4">
-        <v>0.16</v>
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
       <c r="F4">
-        <v>0.1</v>
+        <v>25.32</v>
       </c>
       <c r="G4">
-        <v>153.58</v>
+        <v>16.07</v>
       </c>
       <c r="H4">
-        <v>1.21</v>
+        <v>0.9</v>
       </c>
       <c r="I4">
-        <v>0.5</v>
+        <v>1.09</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>3.4</v>
+      </c>
+      <c r="M4">
+        <v>15.4</v>
+      </c>
+      <c r="N4">
+        <v>3.4</v>
+      </c>
+      <c r="O4">
+        <v>11.29</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
-        <v>72.31999999999999</v>
-      </c>
-      <c r="E5">
-        <v>0.16</v>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
       </c>
       <c r="F5">
-        <v>0.1</v>
+        <v>9167076061667.699</v>
       </c>
       <c r="G5">
-        <v>160.16</v>
+        <v>2.37</v>
       </c>
       <c r="H5">
-        <v>1.23</v>
+        <v>0.9</v>
       </c>
       <c r="I5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>81.2</v>
-      </c>
-      <c r="E6">
-        <v>0.16</v>
-      </c>
-      <c r="F6">
-        <v>0.1</v>
-      </c>
-      <c r="G6">
-        <v>137.65</v>
-      </c>
-      <c r="H6">
-        <v>1.28</v>
-      </c>
-      <c r="I6">
-        <v>0.5</v>
+        <v>1.09</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>13.22</v>
+      </c>
+      <c r="M5">
+        <v>59.96</v>
+      </c>
+      <c r="N5">
+        <v>13.22</v>
+      </c>
+      <c r="O5">
+        <v>59.96</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>-0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.slides draft before discussion with Jonanthan. need to summarize the results and rewrote the conclusion.
</commit_message>
<xml_diff>
--- a/workingfolder/python/tables/NI_Est.xlsx
+++ b/workingfolder/python/tables/NI_Est.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Myworld/Dropbox/ExpProject/workingfolder/python/tables/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476B3B3-DEB6-1E49-B9A7-AD142497355D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="5900" yWindow="6980" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>NI: $\hat\sigma_{pb,SPF}$</t>
   </si>
@@ -52,8 +58,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,17 +115,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -162,7 +182,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,9 +214,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,6 +266,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -403,14 +459,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:Q4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -463,7 +521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -471,87 +529,93 @@
         <v>8</v>
       </c>
       <c r="F2">
-        <v>25.32</v>
+        <v>0.09</v>
       </c>
       <c r="G2">
-        <v>16.07</v>
+        <v>2.77</v>
       </c>
       <c r="H2">
-        <v>0.9</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="I2">
-        <v>1.09</v>
+        <v>1.4079999999999999</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0.91100000000000003</v>
       </c>
       <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="L2" s="2">
         <v>3.4</v>
       </c>
-      <c r="M2">
-        <v>15.4</v>
-      </c>
-      <c r="N2">
+      <c r="M2" s="2">
+        <v>15.39</v>
+      </c>
+      <c r="N2" s="3">
+        <v>3.3974869999999999</v>
+      </c>
+      <c r="O2" s="3">
+        <v>15.394724999999999</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0.99672000000000005</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>2.6543000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>0.09</v>
+      </c>
+      <c r="G3">
+        <v>2.77</v>
+      </c>
+      <c r="H3">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="I3">
+        <v>1.4079999999999999</v>
+      </c>
+      <c r="J3">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="K3">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="L3" s="2">
         <v>3.4</v>
       </c>
-      <c r="O2">
-        <v>11.29</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
+      <c r="M3" s="2">
+        <v>15.39</v>
+      </c>
+      <c r="N3" s="3">
+        <v>3.3974859999999998</v>
+      </c>
+      <c r="O3" s="3">
+        <v>15.394712999999999</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0.99672000000000005</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>2.6543000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <v>471301.73</v>
-      </c>
-      <c r="G3">
-        <v>0.85</v>
-      </c>
-      <c r="H3">
-        <v>-1.74</v>
-      </c>
-      <c r="I3">
-        <v>-0.17</v>
-      </c>
-      <c r="J3">
-        <v>0.91</v>
-      </c>
-      <c r="K3">
-        <v>0.42</v>
-      </c>
-      <c r="L3">
-        <v>168519.46</v>
-      </c>
-      <c r="M3">
-        <v>1.09</v>
-      </c>
-      <c r="N3">
-        <v>0.67</v>
-      </c>
-      <c r="O3">
-        <v>0.58</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -564,94 +628,44 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
       <c r="F4">
-        <v>25.32</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G4">
-        <v>16.07</v>
+        <v>3.85</v>
       </c>
       <c r="H4">
-        <v>0.9</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="I4">
-        <v>1.09</v>
+        <v>1.359</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0.91100000000000003</v>
       </c>
       <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>3.4</v>
-      </c>
-      <c r="M4">
-        <v>15.4</v>
-      </c>
-      <c r="N4">
-        <v>3.4</v>
-      </c>
-      <c r="O4">
-        <v>11.29</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>9167076061667.699</v>
-      </c>
-      <c r="G5">
-        <v>2.37</v>
-      </c>
-      <c r="H5">
-        <v>0.9</v>
-      </c>
-      <c r="I5">
-        <v>1.09</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>13.22</v>
-      </c>
-      <c r="M5">
-        <v>59.96</v>
-      </c>
-      <c r="N5">
-        <v>13.22</v>
-      </c>
-      <c r="O5">
-        <v>59.96</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>-0.03</v>
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="L4" s="2">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="M4" s="2">
+        <v>22.37</v>
+      </c>
+      <c r="N4" s="3">
+        <v>4.8599680000000003</v>
+      </c>
+      <c r="O4" s="3">
+        <v>22.367280000000001</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0.99672099999999997</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>2.6542E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>